<commit_message>
finished vertical profiles adcp vs adv
</commit_message>
<xml_diff>
--- a/data/ADVmeasurements.xlsx
+++ b/data/ADVmeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sjoerd Gn\Documents\Fieldwork\fieldwork-2019-adcp-adv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6618579A-777C-43AC-A995-7805B41A55EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5F970A-7101-4BD8-8EE7-17E2561C9E56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,6 +46,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,6 +62,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,6 +78,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -91,6 +94,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -104,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="27">
   <si>
     <t>Transect #</t>
   </si>
@@ -175,40 +179,16 @@
     <t>-</t>
   </si>
   <si>
-    <t>Group number</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Width of the river [m]</t>
-  </si>
-  <si>
-    <t>Note: is width between the poles</t>
-  </si>
-  <si>
-    <t>Depth at vertical 2 [m]</t>
-  </si>
-  <si>
     <t>location[m]</t>
   </si>
   <si>
-    <t>for 1a 1b and 1c the distance was 24 cm. for 5a 5b 5c 5d the distance is 70 cm</t>
+    <t>Location</t>
   </si>
   <si>
-    <t>for the black and yellow it took a long time to find a steady measurement for every z</t>
+    <t>Depth</t>
   </si>
   <si>
-    <t xml:space="preserve">windy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">upstream of measurement point acceleration water </t>
-  </si>
-  <si>
-    <t xml:space="preserve">!! NOTE ADCP </t>
-  </si>
-  <si>
-    <t>measurement wrongly indicated: started from the right and this is indicated in the software as the left. So the resuts are negative in the discharge and velecoty. Aso the right Q = left Q and other way around</t>
+    <t>unclear</t>
   </si>
 </sst>
 </file>
@@ -218,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,6 +224,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -293,6 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -4273,7 +4260,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4381500" cy="2628900"/>
@@ -4602,7 +4589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="A18:C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5025,36 +5014,17 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="6">
-        <v>43598</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>13.7</v>
-      </c>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>0.57999999999999996</v>
-      </c>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6047,7 +6017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="A17:G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6460,53 +6432,31 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="6">
-        <v>43598</v>
-      </c>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>20.8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>0.56999999999999995</v>
-      </c>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -9092,7 +9042,7 @@
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:I4" si="0">$J$3-B3</f>
@@ -10447,7 +10397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U27" sqref="A17:U27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -10566,7 +10518,7 @@
     </row>
     <row r="4" spans="1:13" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:I4" si="0">$J$3-B3</f>
@@ -10916,37 +10868,25 @@
     </row>
     <row r="17" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="A18" s="7"/>
     </row>
     <row r="19" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="A19" s="7"/>
     </row>
     <row r="20" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A20" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="A20" s="7"/>
     </row>
     <row r="21" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A21" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A21" s="7"/>
     </row>
     <row r="22" spans="1:1" ht="14.25" customHeight="1">
       <c r="A22" s="7"/>
     </row>
     <row r="23" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A23" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="A23" s="7"/>
     </row>
     <row r="24" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A24" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="A24" s="7"/>
     </row>
     <row r="25" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:1" ht="14.25" customHeight="1"/>
@@ -11937,7 +11877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="A17:O22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -12375,39 +12317,17 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B17" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0.31</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0.44</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0.73</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G17" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0.41</v>
-      </c>
-      <c r="I17" s="8">
-        <v>0.34</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="K17" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="L17" s="8">
-        <v>0.19</v>
-      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="18" spans="2:12" ht="14.25" customHeight="1"/>
     <row r="19" spans="2:12" ht="14.25" customHeight="1"/>
@@ -13402,10 +13322,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -13414,7 +13334,7 @@
     <col min="2" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13445,8 +13365,14 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -13477,208 +13403,350 @@
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1">
+    <row r="3" spans="1:12" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>15.74</v>
+      </c>
+      <c r="C4">
+        <v>15.32</v>
+      </c>
+      <c r="D4">
+        <v>14.86</v>
+      </c>
+      <c r="E4">
+        <v>9.48</v>
+      </c>
+      <c r="F4">
+        <v>7.49</v>
+      </c>
+      <c r="G4">
+        <v>5.51</v>
+      </c>
+      <c r="H4">
+        <v>0.81</v>
+      </c>
+      <c r="I4">
+        <v>0.41</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>-0.74</v>
+      </c>
+      <c r="L4">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J5" s="11" t="s">
         <v>22</v>
       </c>
+      <c r="K5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="2">
+    <row r="6" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A6">
         <v>-0.05</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>0.01</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+      <c r="F6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.36</v>
+      </c>
+      <c r="H6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.06</v>
+      </c>
+      <c r="K6">
+        <v>0.08</v>
+      </c>
+      <c r="L6">
+        <v>0.06</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A6" s="2">
+    <row r="7" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A7">
         <v>-0.1</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>0.01</v>
+      </c>
+      <c r="E7">
+        <v>0.08</v>
+      </c>
+      <c r="F7">
+        <v>0.22</v>
+      </c>
+      <c r="G7">
+        <v>0.37</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.08</v>
+      </c>
+      <c r="K7">
+        <v>0.08</v>
+      </c>
+      <c r="L7">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A7" s="2">
+    <row r="8" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A8">
         <v>-0.2</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8">
+        <v>0.02</v>
+      </c>
+      <c r="E8">
+        <v>0.09</v>
+      </c>
+      <c r="F8">
+        <v>0.21</v>
+      </c>
+      <c r="G8">
+        <v>0.34</v>
+      </c>
+      <c r="H8">
+        <v>0.09</v>
+      </c>
+      <c r="I8">
+        <v>0.08</v>
+      </c>
+      <c r="J8">
+        <v>0.08</v>
+      </c>
+      <c r="K8">
+        <v>0.06</v>
+      </c>
+      <c r="L8">
+        <v>0.02</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="2">
+    <row r="9" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A9">
         <v>-0.3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.01</v>
+      </c>
+      <c r="E9">
+        <v>0.09</v>
+      </c>
+      <c r="F9">
+        <v>0.18</v>
+      </c>
+      <c r="G9">
+        <v>0.39</v>
+      </c>
+      <c r="H9">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A9" s="2">
+    <row r="10" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A10">
         <v>-0.4</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="C10">
+        <v>0.04</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.08</v>
+      </c>
+      <c r="F10">
+        <v>0.27</v>
+      </c>
+      <c r="G10">
+        <v>0.35</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="2">
+    <row r="11" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A11">
         <v>-0.5</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="E11">
+        <v>0.08</v>
+      </c>
+      <c r="F11">
+        <v>0.24</v>
+      </c>
+      <c r="G11">
+        <v>0.38</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="2">
+    <row r="12" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A12">
         <v>-0.6</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="E12">
+        <v>0.09</v>
+      </c>
+      <c r="F12">
+        <v>0.15</v>
+      </c>
+      <c r="G12">
+        <v>0.31</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="2">
+    <row r="13" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A13">
         <v>-0.7</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="E13">
+        <v>0.09</v>
+      </c>
+      <c r="F13">
+        <v>0.15</v>
+      </c>
+      <c r="G13">
+        <v>0.28999999999999998</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A13" s="2">
+    <row r="14" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A14">
         <v>-0.8</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A14" s="2">
+    <row r="15" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A15">
         <v>-0.9</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A15" s="2">
+    <row r="16" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A16" s="2">
         <v>-1</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -14663,6 +14731,7 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
finished the issue of these extra distances
</commit_message>
<xml_diff>
--- a/data/ADVmeasurements.xlsx
+++ b/data/ADVmeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sjoerd Gn\Documents\Fieldwork\fieldwork-2019-adcp-adv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5F970A-7101-4BD8-8EE7-17E2561C9E56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF211BB3-6CCA-438A-B316-A86EF3A715EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10398,7 +10398,7 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U27" sqref="A17:U27"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -13325,7 +13325,7 @@
   <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>